<commit_message>
hw4 solved + xlsx done
Signed-off-by: Naveenraj Kamalakannan <therealnaveenkamal@gmail.com>
</commit_message>
<xml_diff>
--- a/xlsx/hw4.xlsx
+++ b/xlsx/hw4.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\keith\source\repos\xlladdins\xll_ml\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Desktop\cpp_course\hw4\xll_ml\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ED5BFD9-3A70-4863-97A7-481AF96E09BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F895D5D-9C56-45B9-AA0D-9E91D8478BCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22276" windowHeight="13996" activeTab="1" xr2:uid="{EDEE3299-5466-402C-8B4F-6E69C4CA67FB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{EDEE3299-5466-402C-8B4F-6E69C4CA67FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Treasury Rates" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Bootstrap" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,9 +34,6 @@
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
-    </ext>
-    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
-      <xlwcv:version setVersion="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -89,12 +87,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
   <si>
     <t>https://home.treasury.gov/resource-center/data-chart-center/interest-rates/daily-treasury-rates.csv/2026/all?field_tdr_date_value=2026&amp;type=daily_treasury_yield_curve&amp;page&amp;_format=csv</t>
-  </si>
-  <si>
-    <t>Add examples for \FI.INSTURMENT, FI.INSTRUMENT, FI.INTRUMENT.ZERO_COUPON_BOND, and FI.INSTRUMENT.BOND</t>
   </si>
   <si>
     <t>Add examples for \FI.CURVE.PWFLAT and FI.CURVE.PWFLAT</t>
@@ -151,22 +146,10 @@
     <t>bill/bond</t>
   </si>
   <si>
-    <t>usd \fi.bond</t>
-  </si>
-  <si>
-    <t>.</t>
-  </si>
-  <si>
     <t>1.5 Mo</t>
   </si>
   <si>
     <t>bootstrap</t>
-  </si>
-  <si>
-    <t>use \fi.zero cupon bond</t>
-  </si>
-  <si>
-    <t>use \fi.ucurve.bootstrap</t>
   </si>
   <si>
     <t>t</t>
@@ -178,19 +161,48 @@
     <t>forward</t>
   </si>
   <si>
-    <t>insert graph</t>
+    <t>FI.INSTRUMENT</t>
   </si>
   <si>
-    <t>plot curve here using pwflate.spot, forward</t>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>ZERO_COUPON_BOND - 2‑year ZCB, payment 1.2</t>
+  </si>
+  <si>
+    <t>BOND -7‑year, 6% coupon, semiannual payments</t>
+  </si>
+  <si>
+    <t>\FI CURVE PWFLAT</t>
+  </si>
+  <si>
+    <t>FI CURVE PWFLAT</t>
+  </si>
+  <si>
+    <t>0.5</t>
+  </si>
+  <si>
+    <t>1.5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="&quot;0x&quot;#"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.00000000000000"/>
+    <numFmt numFmtId="167" formatCode="0.000000000000000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -275,7 +287,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -290,6 +302,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Handle" xfId="3" xr:uid="{FB5D0E3F-B7C2-471A-97B4-EF18ADDF021D}"/>
@@ -297,7 +315,44 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="2" builtinId="10"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="12">
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
@@ -376,6 +431,1920 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Spot Forward chart</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Bootstrap!$J$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>spot</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:glow rad="63500">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="175000"/>
+                    <a:alpha val="25000"/>
+                  </a:schemeClr>
+                </a:glow>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Bootstrap!$I$6:$I$74</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="69"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.30000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.79999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.89999999999999991</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>8.5</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>9.5</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>10.5</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>11.5</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>13.5</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>14.5</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>15.5</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>16.5</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>17.5</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>18.5</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>19.5</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>20.5</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>21.5</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>22.5</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>23.5</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>24.5</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>25.5</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>26.5</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>27.5</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>28.5</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>29.5</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>30</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Bootstrap!$J$6:$J$74</c:f>
+              <c:numCache>
+                <c:formatCode>0.00000000000000</c:formatCode>
+                <c:ptCount val="69"/>
+                <c:pt idx="0">
+                  <c:v>9.4847646038587991E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.9369544121228411E-5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0319493590956648E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0277943078655095E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0138994723094963E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0000018246291529E-4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.8982943137132433E-5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.8256343618716071E-5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.7711393979903836E-5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9.7287544260827642E-5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9.6948464485566675E-5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.3372855440415324E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.5010808928380197E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.507465870831155E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.511722522826579E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.5655466868940493E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.6059148099446527E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.6373122389840105E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3.6624301822154967E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.7286927375230428E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3.783911533612664E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3.8306351303038819E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3.8706839274677829E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3.9262948462946819E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3.9749544002682172E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>4.0178893008331024E-2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>4.0560536568907776E-2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>4.0902007123108028E-2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>4.1209330621888259E-2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>4.186315643180373E-2</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>4.2457543531726878E-2</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>4.3000244796874108E-2</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>4.3497720956592406E-2</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>4.395539902353323E-2</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>4.4377871085324767E-2</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>4.4769048920316926E-2</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>4.5132285481381082E-2</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>4.5470471245130456E-2</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>4.5786111291296547E-2</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>4.6081387463516435E-2</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>4.6358208874972585E-2</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>4.6618253231188969E-2</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>4.686300086056909E-2</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>4.7093762911127483E-2</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>4.7311704847765979E-2</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>4.751786613918077E-2</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>4.7713176836310565E-2</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>4.7898471600254219E-2</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>4.8074501626000701E-2</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>4.8101032464489143E-2</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>4.8126299929716232E-2</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>4.8150392164002534E-2</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>4.817338929673036E-2</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>4.8195364334670289E-2</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>4.8216383936178046E-2</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>4.8236509086557806E-2</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>4.8255795689005086E-2</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>4.82742950831892E-2</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>4.8292054501605959E-2</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>4.8309117472241668E-2</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>4.8325524174775994E-2</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>4.8341311756459983E-2</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>4.835651461289641E-2</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>4.837116463818969E-2</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>4.8385291448293934E-2</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>4.8398922580850649E-2</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>4.8412083674353693E-2</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>4.8424798629093914E-2</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>4.8437089752009464E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3CD8-4481-A1F2-D55D6A698897}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Bootstrap!$K$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>forward</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent2">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:glow rad="63500">
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="175000"/>
+                    <a:alpha val="25000"/>
+                  </a:schemeClr>
+                </a:glow>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Bootstrap!$I$6:$I$74</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="69"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.30000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.79999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.89999999999999991</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>8.5</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>9.5</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>10.5</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>11.5</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>13.5</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>14.5</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>15.5</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>16.5</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>17.5</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>18.5</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>19.5</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>20.5</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>21.5</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>22.5</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>23.5</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>24.5</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>25.5</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>26.5</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>27.5</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>28.5</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>29.5</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>30</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Bootstrap!$K$6:$K$74</c:f>
+              <c:numCache>
+                <c:formatCode>0.000000000000000</c:formatCode>
+                <c:ptCount val="69"/>
+                <c:pt idx="0">
+                  <c:v>9.4847646038587991E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.2197903453443039E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0111459817015834E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0278224291088134E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.4441123390777873E-5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.4441123390777873E-5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.3896746508218072E-5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.3896746508218072E-5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.3896746508218072E-5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9.3896746508218072E-5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9.3896746508218072E-5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6.9924669392274832E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6.9924669392274832E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.5330057828036977E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.5330057828036977E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.8884916712988743E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.8884916712988743E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.8884916712988743E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3.8884916712988743E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4.3913182905984977E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>4.3913182905984977E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>4.3913182905984977E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>4.3913182905984977E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>4.7048477098712585E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>4.7048477098712585E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>4.7048477098712585E-2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>4.7048477098712585E-2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>4.7048477098712585E-2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>4.7048477098712585E-2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>5.493967263011313E-2</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>5.493967263011313E-2</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>5.493967263011313E-2</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>5.493967263011313E-2</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>5.493967263011313E-2</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>5.493967263011313E-2</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>5.493967263011313E-2</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>5.493967263011313E-2</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>5.493967263011313E-2</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>5.493967263011313E-2</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>5.493967263011313E-2</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>5.493967263011313E-2</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>5.493967263011313E-2</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>5.493967263011313E-2</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>5.493967263011313E-2</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>5.493967263011313E-2</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>5.493967263011313E-2</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>5.493967263011313E-2</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>5.493967263011313E-2</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>5.493967263011313E-2</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>4.9162266004027004E-2</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>4.9162266004027004E-2</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>4.9162266004027004E-2</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>4.9162266004027004E-2</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>4.9162266004027004E-2</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>4.9162266004027004E-2</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>4.9162266004027004E-2</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>4.9162266004027004E-2</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>4.9162266004027004E-2</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>4.9162266004027004E-2</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>4.9162266004027004E-2</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>4.9162266004027004E-2</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>4.9162266004027004E-2</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>4.9162266004027004E-2</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>4.9162266004027004E-2</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>4.9162266004027004E-2</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>4.9162266004027004E-2</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>4.9162266004027004E-2</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>4.9162266004027004E-2</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>4.9162266004027004E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-3CD8-4481-A1F2-D55D6A698897}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="133418848"/>
+        <c:axId val="133416928"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="133418848"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                  <a:alpha val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="133416928"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="133416928"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                  <a:alpha val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00000" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="133418848"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="245">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="15000"/>
+        <a:lumOff val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="139700">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="14000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:lumMod val="60000"/>
+          <a:lumOff val="40000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="3"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+            <a:alpha val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="1" kern="1200" cap="none" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>23812</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>404812</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B963100-7EDF-BDC2-B5E8-183F2976C338}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{10D0AB24-5479-4443-82F6-B2817D3A85D2}" name="Table1" displayName="Table1" ref="B4:E5" totalsRowShown="0" headerRowDxfId="11" dataDxfId="6">
+  <autoFilter ref="B4:E5" xr:uid="{10D0AB24-5479-4443-82F6-B2817D3A85D2}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{1C66AA56-0864-45A5-912F-CFB6F2D966E6}" name="1" dataDxfId="10">
+      <calculatedColumnFormula>RAND()</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="2" xr3:uid="{60643C30-37FB-496E-96E2-269B6DA3962E}" name="2" dataDxfId="9">
+      <calculatedColumnFormula>RAND()</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{EC5DA635-09DB-48A1-9492-84C5FCFFF60E}" name="3" dataDxfId="8">
+      <calculatedColumnFormula>RAND()</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{19391DBD-D285-4184-8ABB-327B80A8A763}" name="4" dataDxfId="7">
+      <calculatedColumnFormula>RAND()</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{928AC1D6-F00D-49BD-8F31-870FEB25A547}" name="Table2" displayName="Table2" ref="B4:E5" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+  <autoFilter ref="B4:E5" xr:uid="{928AC1D6-F00D-49BD-8F31-870FEB25A547}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{5E784858-F190-418E-96CE-89E824748BC3}" name="0.5" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{AEDD451D-D200-46AE-B6B5-A18FE25F3884}" name="1" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{0A2AF0F5-A65F-4C53-82F0-C87E57144BB3}" name="1.5" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{30B46E76-DBA7-4A8A-827A-B91642B3DEA5}" name="2" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -698,17 +2667,17 @@
   <dimension ref="B2:P38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B4" t="str">
         <f>_xlfn.WEBSERVICE(B2)</f>
         <v>Date,"1 Mo","1.5 Month","2 Mo","3 Mo","4 Mo","6 Mo","1 Yr","2 Yr","3 Yr","5 Yr","7 Yr","10 Yr","20 Yr","30 Yr"
@@ -746,7 +2715,7 @@
 01/02/2026,3.72,3.71,3.66,3.65,3.62,3.58,3.47,3.47,3.55,3.74,3.95,4.19,4.81,4.86</v>
       </c>
     </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B6" t="str" cm="1">
         <f t="array" ref="B6:P38">_xlfn.TEXTSPLIT(B4,",",CHAR(10))</f>
         <v>Date</v>
@@ -794,7 +2763,7 @@
         <v>"30 Yr"</v>
       </c>
     </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B7" t="str">
         <v>02/18/2026</v>
       </c>
@@ -841,7 +2810,7 @@
         <v>4.71</v>
       </c>
     </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B8" t="str">
         <v>02/17/2026</v>
       </c>
@@ -888,7 +2857,7 @@
         <v>4.68</v>
       </c>
     </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B9" t="str">
         <v>02/13/2026</v>
       </c>
@@ -935,7 +2904,7 @@
         <v>4.69</v>
       </c>
     </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B10" t="str">
         <v>02/12/2026</v>
       </c>
@@ -982,7 +2951,7 @@
         <v>4.72</v>
       </c>
     </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B11" t="str">
         <v>02/11/2026</v>
       </c>
@@ -1029,7 +2998,7 @@
         <v>4.82</v>
       </c>
     </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B12" t="str">
         <v>02/10/2026</v>
       </c>
@@ -1076,7 +3045,7 @@
         <v>4.78</v>
       </c>
     </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B13" t="str">
         <v>02/09/2026</v>
       </c>
@@ -1123,7 +3092,7 @@
         <v>4.85</v>
       </c>
     </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B14" t="str">
         <v>02/06/2026</v>
       </c>
@@ -1170,7 +3139,7 @@
         <v>4.85</v>
       </c>
     </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B15" t="str">
         <v>02/05/2026</v>
       </c>
@@ -1217,7 +3186,7 @@
         <v>4.85</v>
       </c>
     </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B16" t="str">
         <v>02/04/2026</v>
       </c>
@@ -1264,7 +3233,7 @@
         <v>4.91</v>
       </c>
     </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B17" t="str">
         <v>02/03/2026</v>
       </c>
@@ -1311,7 +3280,7 @@
         <v>4.90</v>
       </c>
     </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B18" t="str">
         <v>02/02/2026</v>
       </c>
@@ -1358,7 +3327,7 @@
         <v>4.90</v>
       </c>
     </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B19" t="str">
         <v>01/30/2026</v>
       </c>
@@ -1405,7 +3374,7 @@
         <v>4.87</v>
       </c>
     </row>
-    <row r="20" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B20" t="str">
         <v>01/29/2026</v>
       </c>
@@ -1452,7 +3421,7 @@
         <v>4.85</v>
       </c>
     </row>
-    <row r="21" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B21" t="str">
         <v>01/28/2026</v>
       </c>
@@ -1499,7 +3468,7 @@
         <v>4.85</v>
       </c>
     </row>
-    <row r="22" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B22" t="str">
         <v>01/27/2026</v>
       </c>
@@ -1546,7 +3515,7 @@
         <v>4.83</v>
       </c>
     </row>
-    <row r="23" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B23" t="str">
         <v>01/26/2026</v>
       </c>
@@ -1593,7 +3562,7 @@
         <v>4.80</v>
       </c>
     </row>
-    <row r="24" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B24" t="str">
         <v>01/23/2026</v>
       </c>
@@ -1640,7 +3609,7 @@
         <v>4.82</v>
       </c>
     </row>
-    <row r="25" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B25" t="str">
         <v>01/22/2026</v>
       </c>
@@ -1687,7 +3656,7 @@
         <v>4.84</v>
       </c>
     </row>
-    <row r="26" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B26" t="str">
         <v>01/21/2026</v>
       </c>
@@ -1734,7 +3703,7 @@
         <v>4.87</v>
       </c>
     </row>
-    <row r="27" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B27" t="str">
         <v>01/20/2026</v>
       </c>
@@ -1781,7 +3750,7 @@
         <v>4.91</v>
       </c>
     </row>
-    <row r="28" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B28" t="str">
         <v>01/16/2026</v>
       </c>
@@ -1828,7 +3797,7 @@
         <v>4.83</v>
       </c>
     </row>
-    <row r="29" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B29" t="str">
         <v>01/15/2026</v>
       </c>
@@ -1875,7 +3844,7 @@
         <v>4.79</v>
       </c>
     </row>
-    <row r="30" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B30" t="str">
         <v>01/14/2026</v>
       </c>
@@ -1922,7 +3891,7 @@
         <v>4.79</v>
       </c>
     </row>
-    <row r="31" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B31" t="str">
         <v>01/13/2026</v>
       </c>
@@ -1969,7 +3938,7 @@
         <v>4.83</v>
       </c>
     </row>
-    <row r="32" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B32" t="str">
         <v>01/12/2026</v>
       </c>
@@ -2016,7 +3985,7 @@
         <v>4.83</v>
       </c>
     </row>
-    <row r="33" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B33" t="str">
         <v>01/09/2026</v>
       </c>
@@ -2063,7 +4032,7 @@
         <v>4.82</v>
       </c>
     </row>
-    <row r="34" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B34" t="str">
         <v>01/08/2026</v>
       </c>
@@ -2110,7 +4079,7 @@
         <v>4.85</v>
       </c>
     </row>
-    <row r="35" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B35" t="str">
         <v>01/07/2026</v>
       </c>
@@ -2157,7 +4126,7 @@
         <v>4.82</v>
       </c>
     </row>
-    <row r="36" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B36" t="str">
         <v>01/06/2026</v>
       </c>
@@ -2204,7 +4173,7 @@
         <v>4.86</v>
       </c>
     </row>
-    <row r="37" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B37" t="str">
         <v>01/05/2026</v>
       </c>
@@ -2251,7 +4220,7 @@
         <v>4.85</v>
       </c>
     </row>
-    <row r="38" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B38" t="str">
         <v>01/02/2026</v>
       </c>
@@ -2308,44 +4277,219 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{674E2F35-77D5-4361-8DFB-2603DE31162A}">
-  <dimension ref="B2:B4"/>
+  <dimension ref="B2:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="20.69921875" customWidth="1"/>
+    <col min="3" max="3" width="11.8984375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" s="3" t="s">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B2" s="3"/>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B5" s="3">
+        <f ca="1">RAND()</f>
+        <v>0.68165361828783522</v>
+      </c>
+      <c r="C5" s="3">
+        <f t="shared" ref="C5:E5" ca="1" si="0">RAND()</f>
+        <v>0.58009549984941977</v>
+      </c>
+      <c r="D5" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.80868358712157018</v>
+      </c>
+      <c r="E5" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.30426902985053439</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" cm="1">
+        <f t="array" aca="1" ref="C7" ca="1">_xll.\FI.INSTRUMENT(B4:E4,B5:E5)</f>
+        <v>1718214717344</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" cm="1">
+        <f t="array" aca="1" ref="C8:F9" ca="1">_xll.FI.INSTRUMENT(C7)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B4" s="2"/>
+      <c r="D8">
+        <f ca="1"/>
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <f ca="1"/>
+        <v>3</v>
+      </c>
+      <c r="F8">
+        <f ca="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C9">
+        <f ca="1"/>
+        <v>0.68165361828783522</v>
+      </c>
+      <c r="D9">
+        <f ca="1"/>
+        <v>0.58009549984941977</v>
+      </c>
+      <c r="E9">
+        <f ca="1"/>
+        <v>0.80868358712157018</v>
+      </c>
+      <c r="F9">
+        <f ca="1"/>
+        <v>0.30426902985053439</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="B13" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" cm="1">
+        <f t="array" ref="C13">_xll.\FI.INSTRUMENT.ZERO_COUPON_BOND(2, 1.2)</f>
+        <v>2528401339424</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" ht="56.25" x14ac:dyDescent="0.3">
+      <c r="B14" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" cm="1">
+        <f t="array" ref="C14">_xll.\FI.INSTRUMENT.BOND(7, 0.06, 2)</f>
+        <v>2528309910480</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F354A35E-C248-4AE4-A2E8-7948ED4AA090}">
-  <dimension ref="B2"/>
+  <dimension ref="B2:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="11.8984375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B5" s="3">
+        <v>0.03</v>
+      </c>
+      <c r="C5" s="3">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="D5" s="3">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="E5" s="3">
+        <v>3.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" cm="1">
+        <f t="array" ref="D7">_xll.\FI.CURVE.PWFLAT(B4:E4,B5:E5)</f>
+        <v>1720086463504</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" cm="1">
+        <f t="array" ref="D8:G9">_xll.FI.CURVE.PWFLAT(D7)</f>
+        <v>0.5</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1.5</v>
+      </c>
+      <c r="G8">
         <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="D9">
+        <v>0.03</v>
+      </c>
+      <c r="E9">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="F9">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="G9">
+        <v>3.7999999999999999E-2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -2353,33 +4497,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF2E5B4B-30B9-4C78-A319-DEE69FDAA7AA}">
   <dimension ref="B2:L74"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O27" sqref="O27"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="6" max="6" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.59765625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C2" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="E2" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="F2" t="s">
         <v>18</v>
       </c>
-      <c r="F2" t="s">
-        <v>19</v>
-      </c>
       <c r="G2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+        <v>20</v>
+      </c>
+      <c r="H2" s="9" cm="1">
+        <f t="array" ref="H2">_xll.\FI.CURVE.PWFLAT.BOOTSTRAP(F3:F16, E3:E16)</f>
+        <v>1720091316896</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3" s="4">
         <f>1/12</f>
@@ -2392,13 +4545,14 @@
         <f>1-D3*C3/360</f>
         <v>0.99999141203703701</v>
       </c>
-      <c r="F3" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="F3" s="9" cm="1">
+        <f t="array" ref="F3">_xll.\FI.INSTRUMENT.ZERO_COUPON_BOND(C3)</f>
+        <v>1720091151152</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C4">
         <f>1.5/12</f>
@@ -2411,16 +4565,14 @@
         <f t="shared" ref="E4:E9" si="0">1-D4*C4/360</f>
         <v>0.99998701388888889</v>
       </c>
-      <c r="F4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="F4" s="9" cm="1">
+        <f t="array" ref="F4">_xll.\FI.INSTRUMENT.ZERO_COUPON_BOND(C4)</f>
+        <v>1720090059248</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5" s="4">
         <f>2/12</f>
@@ -2433,22 +4585,23 @@
         <f t="shared" si="0"/>
         <v>0.99998273148148153</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="9" cm="1">
+        <f t="array" ref="F5">_xll.\FI.INSTRUMENT.ZERO_COUPON_BOND(C5)</f>
+        <v>1720090061984</v>
+      </c>
+      <c r="I5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="I5" s="7" t="s">
-        <v>26</v>
-      </c>
       <c r="J5" s="7" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="K5" s="7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6">
         <f>3/12</f>
@@ -2461,8 +4614,9 @@
         <f t="shared" si="0"/>
         <v>0.99997430555555555</v>
       </c>
-      <c r="F6" t="s">
-        <v>21</v>
+      <c r="F6" s="9" cm="1">
+        <f t="array" ref="F6">_xll.\FI.INSTRUMENT.ZERO_COUPON_BOND(C6)</f>
+        <v>1720090064000</v>
       </c>
       <c r="H6">
         <v>0.1</v>
@@ -2471,10 +4625,18 @@
         <f t="array" ref="I6:I74">_xlfn.VSTACK(_xlfn.SEQUENCE(1/H6,1,0,H6),_xlfn.SEQUENCE(1+29/H7,1,1,H7))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="J6" s="10" cm="1">
+        <f t="array" ref="J6">_xll.FI.CURVE.SPOT($H$2,I6)</f>
+        <v>9.4847646038587991E-5</v>
+      </c>
+      <c r="K6" s="11" cm="1">
+        <f t="array" ref="K6">_xll.FI.CURVE.FORWARD($H$2,I6)</f>
+        <v>9.4847646038587991E-5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" s="5">
         <f>4/12</f>
@@ -2487,8 +4649,9 @@
         <f t="shared" si="0"/>
         <v>0.99996574074074074</v>
       </c>
-      <c r="F7" t="s">
-        <v>21</v>
+      <c r="F7" s="9" cm="1">
+        <f t="array" ref="F7">_xll.\FI.INSTRUMENT.ZERO_COUPON_BOND(C7)</f>
+        <v>1720091301056</v>
       </c>
       <c r="H7">
         <v>0.5</v>
@@ -2496,10 +4659,18 @@
       <c r="I7">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="J7" s="10" cm="1">
+        <f t="array" ref="J7">_xll.FI.CURVE.SPOT($H$2,I7)</f>
+        <v>9.9369544121228411E-5</v>
+      </c>
+      <c r="K7" s="11" cm="1">
+        <f t="array" ref="K7">_xll.FI.CURVE.FORWARD($H$2,I7)</f>
+        <v>1.2197903453443039E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C8">
         <f>6/12</f>
@@ -2512,16 +4683,25 @@
         <f t="shared" si="0"/>
         <v>0.99995000000000001</v>
       </c>
-      <c r="F8" t="s">
-        <v>21</v>
+      <c r="F8" s="9" cm="1">
+        <f t="array" ref="F8">_xll.\FI.INSTRUMENT.ZERO_COUPON_BOND(C8)</f>
+        <v>1720091147552</v>
       </c>
       <c r="I8">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="J8" s="10" cm="1">
+        <f t="array" ref="J8">_xll.FI.CURVE.SPOT($H$2,I8)</f>
+        <v>1.0319493590956648E-4</v>
+      </c>
+      <c r="K8" s="11" cm="1">
+        <f t="array" ref="K8">_xll.FI.CURVE.FORWARD($H$2,I8)</f>
+        <v>1.0111459817015834E-4</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -2533,19 +4713,26 @@
         <f t="shared" si="0"/>
         <v>0.99990305555555559</v>
       </c>
-      <c r="F9" t="s">
-        <v>21</v>
+      <c r="F9" s="9" cm="1">
+        <f t="array" ref="F9">_xll.\FI.INSTRUMENT.ZERO_COUPON_BOND(C9)</f>
+        <v>1719619866752</v>
       </c>
       <c r="I9">
         <v>0.30000000000000004</v>
       </c>
-      <c r="L9" s="6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="J9" s="10" cm="1">
+        <f t="array" ref="J9">_xll.FI.CURVE.SPOT($H$2,I9)</f>
+        <v>1.0277943078655095E-4</v>
+      </c>
+      <c r="K9" s="11" cm="1">
+        <f t="array" ref="K9">_xll.FI.CURVE.FORWARD($H$2,I9)</f>
+        <v>1.0278224291088134E-4</v>
+      </c>
+      <c r="L9" s="6"/>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10">
         <v>2</v>
@@ -2556,16 +4743,25 @@
       <c r="E10">
         <v>1</v>
       </c>
-      <c r="F10" s="6" t="s">
-        <v>20</v>
+      <c r="F10" s="9" cm="1">
+        <f t="array" ref="F10">_xll.\FI.INSTRUMENT.BOND(C10,D10,2)</f>
+        <v>1719837818736</v>
       </c>
       <c r="I10">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="J10" s="10" cm="1">
+        <f t="array" ref="J10">_xll.FI.CURVE.SPOT($H$2,I10)</f>
+        <v>1.0138994723094963E-4</v>
+      </c>
+      <c r="K10" s="11" cm="1">
+        <f t="array" ref="K10">_xll.FI.CURVE.FORWARD($H$2,I10)</f>
+        <v>9.4441123390777873E-5</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C11">
         <v>3</v>
@@ -2576,16 +4772,25 @@
       <c r="E11">
         <v>1</v>
       </c>
-      <c r="F11" t="s">
-        <v>21</v>
+      <c r="F11" s="9" cm="1">
+        <f t="array" ref="F11">_xll.\FI.INSTRUMENT.BOND(C11,D11,2)</f>
+        <v>1719619276864</v>
       </c>
       <c r="I11">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="J11" s="10" cm="1">
+        <f t="array" ref="J11">_xll.FI.CURVE.SPOT($H$2,I11)</f>
+        <v>1.0000018246291529E-4</v>
+      </c>
+      <c r="K11" s="11" cm="1">
+        <f t="array" ref="K11">_xll.FI.CURVE.FORWARD($H$2,I11)</f>
+        <v>9.4441123390777873E-5</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B12" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C12">
         <v>5</v>
@@ -2596,16 +4801,25 @@
       <c r="E12">
         <v>1</v>
       </c>
-      <c r="F12" t="s">
-        <v>21</v>
+      <c r="F12" s="9" cm="1">
+        <f t="array" ref="F12">_xll.\FI.INSTRUMENT.BOND(C12,D12,2)</f>
+        <v>1719837814416</v>
       </c>
       <c r="I12">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="J12" s="10" cm="1">
+        <f t="array" ref="J12">_xll.FI.CURVE.SPOT($H$2,I12)</f>
+        <v>9.8982943137132433E-5</v>
+      </c>
+      <c r="K12" s="11" cm="1">
+        <f t="array" ref="K12">_xll.FI.CURVE.FORWARD($H$2,I12)</f>
+        <v>9.3896746508218072E-5</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C13">
         <v>7</v>
@@ -2616,16 +4830,25 @@
       <c r="E13">
         <v>1</v>
       </c>
-      <c r="F13" t="s">
-        <v>21</v>
+      <c r="F13" s="9" cm="1">
+        <f t="array" ref="F13">_xll.\FI.INSTRUMENT.BOND(C13,D13,2)</f>
+        <v>1719837821616</v>
       </c>
       <c r="I13">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="J13" s="10" cm="1">
+        <f t="array" ref="J13">_xll.FI.CURVE.SPOT($H$2,I13)</f>
+        <v>9.8256343618716071E-5</v>
+      </c>
+      <c r="K13" s="11" cm="1">
+        <f t="array" ref="K13">_xll.FI.CURVE.FORWARD($H$2,I13)</f>
+        <v>9.3896746508218072E-5</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C14">
         <v>10</v>
@@ -2636,16 +4859,25 @@
       <c r="E14">
         <v>1</v>
       </c>
-      <c r="F14" t="s">
-        <v>21</v>
+      <c r="F14" s="9" cm="1">
+        <f t="array" ref="F14">_xll.\FI.INSTRUMENT.BOND(C14,D14,2)</f>
+        <v>1719837828336</v>
       </c>
       <c r="I14">
         <v>0.79999999999999993</v>
       </c>
-    </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="J14" s="10" cm="1">
+        <f t="array" ref="J14">_xll.FI.CURVE.SPOT($H$2,I14)</f>
+        <v>9.7711393979903836E-5</v>
+      </c>
+      <c r="K14" s="11" cm="1">
+        <f t="array" ref="K14">_xll.FI.CURVE.FORWARD($H$2,I14)</f>
+        <v>9.3896746508218072E-5</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B15" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C15">
         <v>20</v>
@@ -2656,16 +4888,25 @@
       <c r="E15">
         <v>1</v>
       </c>
-      <c r="F15" t="s">
-        <v>21</v>
+      <c r="F15" s="9" cm="1">
+        <f t="array" ref="F15">_xll.\FI.INSTRUMENT.BOND(C15,D15,2)</f>
+        <v>1719837818576</v>
       </c>
       <c r="I15">
         <v>0.89999999999999991</v>
       </c>
-    </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="J15" s="10" cm="1">
+        <f t="array" ref="J15">_xll.FI.CURVE.SPOT($H$2,I15)</f>
+        <v>9.7287544260827642E-5</v>
+      </c>
+      <c r="K15" s="11" cm="1">
+        <f t="array" ref="K15">_xll.FI.CURVE.FORWARD($H$2,I15)</f>
+        <v>9.3896746508218072E-5</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B16" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C16">
         <v>30</v>
@@ -2676,301 +4917,775 @@
       <c r="E16">
         <v>1</v>
       </c>
-      <c r="F16" t="s">
-        <v>21</v>
+      <c r="F16" s="9" cm="1">
+        <f t="array" ref="F16">_xll.\FI.INSTRUMENT.BOND(C16,D16,2)</f>
+        <v>1719837823856</v>
       </c>
       <c r="I16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="9:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="J16" s="10" cm="1">
+        <f t="array" ref="J16">_xll.FI.CURVE.SPOT($H$2,I16)</f>
+        <v>9.6948464485566675E-5</v>
+      </c>
+      <c r="K16" s="11" cm="1">
+        <f t="array" ref="K16">_xll.FI.CURVE.FORWARD($H$2,I16)</f>
+        <v>9.3896746508218072E-5</v>
+      </c>
+    </row>
+    <row r="17" spans="6:11" x14ac:dyDescent="0.3">
       <c r="I17">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="18" spans="9:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="J17" s="10" cm="1">
+        <f t="array" ref="J17">_xll.FI.CURVE.SPOT($H$2,I17)</f>
+        <v>2.3372855440415324E-2</v>
+      </c>
+      <c r="K17" s="11" cm="1">
+        <f t="array" ref="K17">_xll.FI.CURVE.FORWARD($H$2,I17)</f>
+        <v>6.9924669392274832E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="6:11" x14ac:dyDescent="0.3">
       <c r="I18">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="9:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="J18" s="10" cm="1">
+        <f t="array" ref="J18">_xll.FI.CURVE.SPOT($H$2,I18)</f>
+        <v>3.5010808928380197E-2</v>
+      </c>
+      <c r="K18" s="11" cm="1">
+        <f t="array" ref="K18">_xll.FI.CURVE.FORWARD($H$2,I18)</f>
+        <v>6.9924669392274832E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="6:11" x14ac:dyDescent="0.3">
       <c r="I19">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="20" spans="9:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="J19" s="10" cm="1">
+        <f t="array" ref="J19">_xll.FI.CURVE.SPOT($H$2,I19)</f>
+        <v>3.507465870831155E-2</v>
+      </c>
+      <c r="K19" s="11" cm="1">
+        <f t="array" ref="K19">_xll.FI.CURVE.FORWARD($H$2,I19)</f>
+        <v>3.5330057828036977E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="6:11" x14ac:dyDescent="0.3">
       <c r="I20">
         <v>3</v>
       </c>
-    </row>
-    <row r="21" spans="9:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="J20" s="10" cm="1">
+        <f t="array" ref="J20">_xll.FI.CURVE.SPOT($H$2,I20)</f>
+        <v>3.511722522826579E-2</v>
+      </c>
+      <c r="K20" s="11" cm="1">
+        <f t="array" ref="K20">_xll.FI.CURVE.FORWARD($H$2,I20)</f>
+        <v>3.5330057828036977E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="6:11" x14ac:dyDescent="0.3">
+      <c r="F21" s="5"/>
       <c r="I21">
         <v>3.5</v>
       </c>
-    </row>
-    <row r="22" spans="9:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="J21" s="10" cm="1">
+        <f t="array" ref="J21">_xll.FI.CURVE.SPOT($H$2,I21)</f>
+        <v>3.5655466868940493E-2</v>
+      </c>
+      <c r="K21" s="11" cm="1">
+        <f t="array" ref="K21">_xll.FI.CURVE.FORWARD($H$2,I21)</f>
+        <v>3.8884916712988743E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="6:11" x14ac:dyDescent="0.3">
       <c r="I22">
         <v>4</v>
       </c>
-    </row>
-    <row r="23" spans="9:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="J22" s="10" cm="1">
+        <f t="array" ref="J22">_xll.FI.CURVE.SPOT($H$2,I22)</f>
+        <v>3.6059148099446527E-2</v>
+      </c>
+      <c r="K22" s="11" cm="1">
+        <f t="array" ref="K22">_xll.FI.CURVE.FORWARD($H$2,I22)</f>
+        <v>3.8884916712988743E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="6:11" x14ac:dyDescent="0.3">
       <c r="I23">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="24" spans="9:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="J23" s="10" cm="1">
+        <f t="array" ref="J23">_xll.FI.CURVE.SPOT($H$2,I23)</f>
+        <v>3.6373122389840105E-2</v>
+      </c>
+      <c r="K23" s="11" cm="1">
+        <f t="array" ref="K23">_xll.FI.CURVE.FORWARD($H$2,I23)</f>
+        <v>3.8884916712988743E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="6:11" x14ac:dyDescent="0.3">
       <c r="I24">
         <v>5</v>
       </c>
-    </row>
-    <row r="25" spans="9:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="J24" s="10" cm="1">
+        <f t="array" ref="J24">_xll.FI.CURVE.SPOT($H$2,I24)</f>
+        <v>3.6624301822154967E-2</v>
+      </c>
+      <c r="K24" s="11" cm="1">
+        <f t="array" ref="K24">_xll.FI.CURVE.FORWARD($H$2,I24)</f>
+        <v>3.8884916712988743E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="6:11" x14ac:dyDescent="0.3">
       <c r="I25">
         <v>5.5</v>
       </c>
-    </row>
-    <row r="26" spans="9:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="J25" s="10" cm="1">
+        <f t="array" ref="J25">_xll.FI.CURVE.SPOT($H$2,I25)</f>
+        <v>3.7286927375230428E-2</v>
+      </c>
+      <c r="K25" s="11" cm="1">
+        <f t="array" ref="K25">_xll.FI.CURVE.FORWARD($H$2,I25)</f>
+        <v>4.3913182905984977E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="6:11" x14ac:dyDescent="0.3">
       <c r="I26">
         <v>6</v>
       </c>
-    </row>
-    <row r="27" spans="9:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="J26" s="10" cm="1">
+        <f t="array" ref="J26">_xll.FI.CURVE.SPOT($H$2,I26)</f>
+        <v>3.783911533612664E-2</v>
+      </c>
+      <c r="K26" s="11" cm="1">
+        <f t="array" ref="K26">_xll.FI.CURVE.FORWARD($H$2,I26)</f>
+        <v>4.3913182905984977E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="6:11" x14ac:dyDescent="0.3">
       <c r="I27">
         <v>6.5</v>
       </c>
-    </row>
-    <row r="28" spans="9:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="J27" s="10" cm="1">
+        <f t="array" ref="J27">_xll.FI.CURVE.SPOT($H$2,I27)</f>
+        <v>3.8306351303038819E-2</v>
+      </c>
+      <c r="K27" s="11" cm="1">
+        <f t="array" ref="K27">_xll.FI.CURVE.FORWARD($H$2,I27)</f>
+        <v>4.3913182905984977E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="6:11" x14ac:dyDescent="0.3">
       <c r="I28">
         <v>7</v>
       </c>
-    </row>
-    <row r="29" spans="9:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="J28" s="10" cm="1">
+        <f t="array" ref="J28">_xll.FI.CURVE.SPOT($H$2,I28)</f>
+        <v>3.8706839274677829E-2</v>
+      </c>
+      <c r="K28" s="11" cm="1">
+        <f t="array" ref="K28">_xll.FI.CURVE.FORWARD($H$2,I28)</f>
+        <v>4.3913182905984977E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="6:11" x14ac:dyDescent="0.3">
       <c r="I29">
         <v>7.5</v>
       </c>
-    </row>
-    <row r="30" spans="9:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="J29" s="10" cm="1">
+        <f t="array" ref="J29">_xll.FI.CURVE.SPOT($H$2,I29)</f>
+        <v>3.9262948462946819E-2</v>
+      </c>
+      <c r="K29" s="11" cm="1">
+        <f t="array" ref="K29">_xll.FI.CURVE.FORWARD($H$2,I29)</f>
+        <v>4.7048477098712585E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="6:11" x14ac:dyDescent="0.3">
       <c r="I30">
         <v>8</v>
       </c>
-    </row>
-    <row r="31" spans="9:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="J30" s="10" cm="1">
+        <f t="array" ref="J30">_xll.FI.CURVE.SPOT($H$2,I30)</f>
+        <v>3.9749544002682172E-2</v>
+      </c>
+      <c r="K30" s="11" cm="1">
+        <f t="array" ref="K30">_xll.FI.CURVE.FORWARD($H$2,I30)</f>
+        <v>4.7048477098712585E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="6:11" x14ac:dyDescent="0.3">
       <c r="I31">
         <v>8.5</v>
       </c>
-    </row>
-    <row r="32" spans="9:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="J31" s="10" cm="1">
+        <f t="array" ref="J31">_xll.FI.CURVE.SPOT($H$2,I31)</f>
+        <v>4.0178893008331024E-2</v>
+      </c>
+      <c r="K31" s="11" cm="1">
+        <f t="array" ref="K31">_xll.FI.CURVE.FORWARD($H$2,I31)</f>
+        <v>4.7048477098712585E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="6:11" x14ac:dyDescent="0.3">
       <c r="I32">
         <v>9</v>
       </c>
-    </row>
-    <row r="33" spans="9:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="J32" s="10" cm="1">
+        <f t="array" ref="J32">_xll.FI.CURVE.SPOT($H$2,I32)</f>
+        <v>4.0560536568907776E-2</v>
+      </c>
+      <c r="K32" s="11" cm="1">
+        <f t="array" ref="K32">_xll.FI.CURVE.FORWARD($H$2,I32)</f>
+        <v>4.7048477098712585E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="9:11" x14ac:dyDescent="0.3">
       <c r="I33">
         <v>9.5</v>
       </c>
-    </row>
-    <row r="34" spans="9:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="J33" s="10" cm="1">
+        <f t="array" ref="J33">_xll.FI.CURVE.SPOT($H$2,I33)</f>
+        <v>4.0902007123108028E-2</v>
+      </c>
+      <c r="K33" s="11" cm="1">
+        <f t="array" ref="K33">_xll.FI.CURVE.FORWARD($H$2,I33)</f>
+        <v>4.7048477098712585E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="9:11" x14ac:dyDescent="0.3">
       <c r="I34">
         <v>10</v>
       </c>
-    </row>
-    <row r="35" spans="9:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="J34" s="10" cm="1">
+        <f t="array" ref="J34">_xll.FI.CURVE.SPOT($H$2,I34)</f>
+        <v>4.1209330621888259E-2</v>
+      </c>
+      <c r="K34" s="11" cm="1">
+        <f t="array" ref="K34">_xll.FI.CURVE.FORWARD($H$2,I34)</f>
+        <v>4.7048477098712585E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="9:11" x14ac:dyDescent="0.3">
       <c r="I35">
         <v>10.5</v>
       </c>
-    </row>
-    <row r="36" spans="9:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="J35" s="10" cm="1">
+        <f t="array" ref="J35">_xll.FI.CURVE.SPOT($H$2,I35)</f>
+        <v>4.186315643180373E-2</v>
+      </c>
+      <c r="K35" s="11" cm="1">
+        <f t="array" ref="K35">_xll.FI.CURVE.FORWARD($H$2,I35)</f>
+        <v>5.493967263011313E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="9:11" x14ac:dyDescent="0.3">
       <c r="I36">
         <v>11</v>
       </c>
-    </row>
-    <row r="37" spans="9:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="J36" s="10" cm="1">
+        <f t="array" ref="J36">_xll.FI.CURVE.SPOT($H$2,I36)</f>
+        <v>4.2457543531726878E-2</v>
+      </c>
+      <c r="K36" s="11" cm="1">
+        <f t="array" ref="K36">_xll.FI.CURVE.FORWARD($H$2,I36)</f>
+        <v>5.493967263011313E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="9:11" x14ac:dyDescent="0.3">
       <c r="I37">
         <v>11.5</v>
       </c>
-    </row>
-    <row r="38" spans="9:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="J37" s="10" cm="1">
+        <f t="array" ref="J37">_xll.FI.CURVE.SPOT($H$2,I37)</f>
+        <v>4.3000244796874108E-2</v>
+      </c>
+      <c r="K37" s="11" cm="1">
+        <f t="array" ref="K37">_xll.FI.CURVE.FORWARD($H$2,I37)</f>
+        <v>5.493967263011313E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="9:11" x14ac:dyDescent="0.3">
       <c r="I38">
         <v>12</v>
       </c>
-    </row>
-    <row r="39" spans="9:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="J38" s="10" cm="1">
+        <f t="array" ref="J38">_xll.FI.CURVE.SPOT($H$2,I38)</f>
+        <v>4.3497720956592406E-2</v>
+      </c>
+      <c r="K38" s="11" cm="1">
+        <f t="array" ref="K38">_xll.FI.CURVE.FORWARD($H$2,I38)</f>
+        <v>5.493967263011313E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="9:11" x14ac:dyDescent="0.3">
       <c r="I39">
         <v>12.5</v>
       </c>
-    </row>
-    <row r="40" spans="9:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="J39" s="10" cm="1">
+        <f t="array" ref="J39">_xll.FI.CURVE.SPOT($H$2,I39)</f>
+        <v>4.395539902353323E-2</v>
+      </c>
+      <c r="K39" s="11" cm="1">
+        <f t="array" ref="K39">_xll.FI.CURVE.FORWARD($H$2,I39)</f>
+        <v>5.493967263011313E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="9:11" x14ac:dyDescent="0.3">
       <c r="I40">
         <v>13</v>
       </c>
-    </row>
-    <row r="41" spans="9:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="J40" s="10" cm="1">
+        <f t="array" ref="J40">_xll.FI.CURVE.SPOT($H$2,I40)</f>
+        <v>4.4377871085324767E-2</v>
+      </c>
+      <c r="K40" s="11" cm="1">
+        <f t="array" ref="K40">_xll.FI.CURVE.FORWARD($H$2,I40)</f>
+        <v>5.493967263011313E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="9:11" x14ac:dyDescent="0.3">
       <c r="I41">
         <v>13.5</v>
       </c>
-    </row>
-    <row r="42" spans="9:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="J41" s="10" cm="1">
+        <f t="array" ref="J41">_xll.FI.CURVE.SPOT($H$2,I41)</f>
+        <v>4.4769048920316926E-2</v>
+      </c>
+      <c r="K41" s="11" cm="1">
+        <f t="array" ref="K41">_xll.FI.CURVE.FORWARD($H$2,I41)</f>
+        <v>5.493967263011313E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="9:11" x14ac:dyDescent="0.3">
       <c r="I42">
         <v>14</v>
       </c>
-    </row>
-    <row r="43" spans="9:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="J42" s="10" cm="1">
+        <f t="array" ref="J42">_xll.FI.CURVE.SPOT($H$2,I42)</f>
+        <v>4.5132285481381082E-2</v>
+      </c>
+      <c r="K42" s="11" cm="1">
+        <f t="array" ref="K42">_xll.FI.CURVE.FORWARD($H$2,I42)</f>
+        <v>5.493967263011313E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="9:11" x14ac:dyDescent="0.3">
       <c r="I43">
         <v>14.5</v>
       </c>
-    </row>
-    <row r="44" spans="9:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="J43" s="10" cm="1">
+        <f t="array" ref="J43">_xll.FI.CURVE.SPOT($H$2,I43)</f>
+        <v>4.5470471245130456E-2</v>
+      </c>
+      <c r="K43" s="11" cm="1">
+        <f t="array" ref="K43">_xll.FI.CURVE.FORWARD($H$2,I43)</f>
+        <v>5.493967263011313E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="9:11" x14ac:dyDescent="0.3">
       <c r="I44">
         <v>15</v>
       </c>
-    </row>
-    <row r="45" spans="9:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="J44" s="10" cm="1">
+        <f t="array" ref="J44">_xll.FI.CURVE.SPOT($H$2,I44)</f>
+        <v>4.5786111291296547E-2</v>
+      </c>
+      <c r="K44" s="11" cm="1">
+        <f t="array" ref="K44">_xll.FI.CURVE.FORWARD($H$2,I44)</f>
+        <v>5.493967263011313E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="9:11" x14ac:dyDescent="0.3">
       <c r="I45">
         <v>15.5</v>
       </c>
-    </row>
-    <row r="46" spans="9:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="J45" s="10" cm="1">
+        <f t="array" ref="J45">_xll.FI.CURVE.SPOT($H$2,I45)</f>
+        <v>4.6081387463516435E-2</v>
+      </c>
+      <c r="K45" s="11" cm="1">
+        <f t="array" ref="K45">_xll.FI.CURVE.FORWARD($H$2,I45)</f>
+        <v>5.493967263011313E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="9:11" x14ac:dyDescent="0.3">
       <c r="I46">
         <v>16</v>
       </c>
-    </row>
-    <row r="47" spans="9:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="J46" s="10" cm="1">
+        <f t="array" ref="J46">_xll.FI.CURVE.SPOT($H$2,I46)</f>
+        <v>4.6358208874972585E-2</v>
+      </c>
+      <c r="K46" s="11" cm="1">
+        <f t="array" ref="K46">_xll.FI.CURVE.FORWARD($H$2,I46)</f>
+        <v>5.493967263011313E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="9:11" x14ac:dyDescent="0.3">
       <c r="I47">
         <v>16.5</v>
       </c>
-    </row>
-    <row r="48" spans="9:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="J47" s="10" cm="1">
+        <f t="array" ref="J47">_xll.FI.CURVE.SPOT($H$2,I47)</f>
+        <v>4.6618253231188969E-2</v>
+      </c>
+      <c r="K47" s="11" cm="1">
+        <f t="array" ref="K47">_xll.FI.CURVE.FORWARD($H$2,I47)</f>
+        <v>5.493967263011313E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="9:11" x14ac:dyDescent="0.3">
       <c r="I48">
         <v>17</v>
       </c>
-    </row>
-    <row r="49" spans="9:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="J48" s="10" cm="1">
+        <f t="array" ref="J48">_xll.FI.CURVE.SPOT($H$2,I48)</f>
+        <v>4.686300086056909E-2</v>
+      </c>
+      <c r="K48" s="11" cm="1">
+        <f t="array" ref="K48">_xll.FI.CURVE.FORWARD($H$2,I48)</f>
+        <v>5.493967263011313E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="9:11" x14ac:dyDescent="0.3">
       <c r="I49">
         <v>17.5</v>
       </c>
-    </row>
-    <row r="50" spans="9:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="J49" s="10" cm="1">
+        <f t="array" ref="J49">_xll.FI.CURVE.SPOT($H$2,I49)</f>
+        <v>4.7093762911127483E-2</v>
+      </c>
+      <c r="K49" s="11" cm="1">
+        <f t="array" ref="K49">_xll.FI.CURVE.FORWARD($H$2,I49)</f>
+        <v>5.493967263011313E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="9:11" x14ac:dyDescent="0.3">
       <c r="I50">
         <v>18</v>
       </c>
-    </row>
-    <row r="51" spans="9:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="J50" s="10" cm="1">
+        <f t="array" ref="J50">_xll.FI.CURVE.SPOT($H$2,I50)</f>
+        <v>4.7311704847765979E-2</v>
+      </c>
+      <c r="K50" s="11" cm="1">
+        <f t="array" ref="K50">_xll.FI.CURVE.FORWARD($H$2,I50)</f>
+        <v>5.493967263011313E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="9:11" x14ac:dyDescent="0.3">
       <c r="I51">
         <v>18.5</v>
       </c>
-    </row>
-    <row r="52" spans="9:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="J51" s="10" cm="1">
+        <f t="array" ref="J51">_xll.FI.CURVE.SPOT($H$2,I51)</f>
+        <v>4.751786613918077E-2</v>
+      </c>
+      <c r="K51" s="11" cm="1">
+        <f t="array" ref="K51">_xll.FI.CURVE.FORWARD($H$2,I51)</f>
+        <v>5.493967263011313E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="9:11" x14ac:dyDescent="0.3">
       <c r="I52">
         <v>19</v>
       </c>
-    </row>
-    <row r="53" spans="9:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="J52" s="10" cm="1">
+        <f t="array" ref="J52">_xll.FI.CURVE.SPOT($H$2,I52)</f>
+        <v>4.7713176836310565E-2</v>
+      </c>
+      <c r="K52" s="11" cm="1">
+        <f t="array" ref="K52">_xll.FI.CURVE.FORWARD($H$2,I52)</f>
+        <v>5.493967263011313E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="9:11" x14ac:dyDescent="0.3">
       <c r="I53">
         <v>19.5</v>
       </c>
-    </row>
-    <row r="54" spans="9:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="J53" s="10" cm="1">
+        <f t="array" ref="J53">_xll.FI.CURVE.SPOT($H$2,I53)</f>
+        <v>4.7898471600254219E-2</v>
+      </c>
+      <c r="K53" s="11" cm="1">
+        <f t="array" ref="K53">_xll.FI.CURVE.FORWARD($H$2,I53)</f>
+        <v>5.493967263011313E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="9:11" x14ac:dyDescent="0.3">
       <c r="I54">
         <v>20</v>
       </c>
-    </row>
-    <row r="55" spans="9:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="J54" s="10" cm="1">
+        <f t="array" ref="J54">_xll.FI.CURVE.SPOT($H$2,I54)</f>
+        <v>4.8074501626000701E-2</v>
+      </c>
+      <c r="K54" s="11" cm="1">
+        <f t="array" ref="K54">_xll.FI.CURVE.FORWARD($H$2,I54)</f>
+        <v>5.493967263011313E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="9:11" x14ac:dyDescent="0.3">
       <c r="I55">
         <v>20.5</v>
       </c>
-    </row>
-    <row r="56" spans="9:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="J55" s="10" cm="1">
+        <f t="array" ref="J55">_xll.FI.CURVE.SPOT($H$2,I55)</f>
+        <v>4.8101032464489143E-2</v>
+      </c>
+      <c r="K55" s="11" cm="1">
+        <f t="array" ref="K55">_xll.FI.CURVE.FORWARD($H$2,I55)</f>
+        <v>4.9162266004027004E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="9:11" x14ac:dyDescent="0.3">
       <c r="I56">
         <v>21</v>
       </c>
-    </row>
-    <row r="57" spans="9:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="J56" s="10" cm="1">
+        <f t="array" ref="J56">_xll.FI.CURVE.SPOT($H$2,I56)</f>
+        <v>4.8126299929716232E-2</v>
+      </c>
+      <c r="K56" s="11" cm="1">
+        <f t="array" ref="K56">_xll.FI.CURVE.FORWARD($H$2,I56)</f>
+        <v>4.9162266004027004E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="9:11" x14ac:dyDescent="0.3">
       <c r="I57">
         <v>21.5</v>
       </c>
-    </row>
-    <row r="58" spans="9:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="J57" s="10" cm="1">
+        <f t="array" ref="J57">_xll.FI.CURVE.SPOT($H$2,I57)</f>
+        <v>4.8150392164002534E-2</v>
+      </c>
+      <c r="K57" s="11" cm="1">
+        <f t="array" ref="K57">_xll.FI.CURVE.FORWARD($H$2,I57)</f>
+        <v>4.9162266004027004E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="9:11" x14ac:dyDescent="0.3">
       <c r="I58">
         <v>22</v>
       </c>
-    </row>
-    <row r="59" spans="9:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="J58" s="10" cm="1">
+        <f t="array" ref="J58">_xll.FI.CURVE.SPOT($H$2,I58)</f>
+        <v>4.817338929673036E-2</v>
+      </c>
+      <c r="K58" s="11" cm="1">
+        <f t="array" ref="K58">_xll.FI.CURVE.FORWARD($H$2,I58)</f>
+        <v>4.9162266004027004E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="9:11" x14ac:dyDescent="0.3">
       <c r="I59">
         <v>22.5</v>
       </c>
-    </row>
-    <row r="60" spans="9:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="J59" s="10" cm="1">
+        <f t="array" ref="J59">_xll.FI.CURVE.SPOT($H$2,I59)</f>
+        <v>4.8195364334670289E-2</v>
+      </c>
+      <c r="K59" s="11" cm="1">
+        <f t="array" ref="K59">_xll.FI.CURVE.FORWARD($H$2,I59)</f>
+        <v>4.9162266004027004E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="9:11" x14ac:dyDescent="0.3">
       <c r="I60">
         <v>23</v>
       </c>
-    </row>
-    <row r="61" spans="9:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="J60" s="10" cm="1">
+        <f t="array" ref="J60">_xll.FI.CURVE.SPOT($H$2,I60)</f>
+        <v>4.8216383936178046E-2</v>
+      </c>
+      <c r="K60" s="11" cm="1">
+        <f t="array" ref="K60">_xll.FI.CURVE.FORWARD($H$2,I60)</f>
+        <v>4.9162266004027004E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="9:11" x14ac:dyDescent="0.3">
       <c r="I61">
         <v>23.5</v>
       </c>
-    </row>
-    <row r="62" spans="9:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="J61" s="10" cm="1">
+        <f t="array" ref="J61">_xll.FI.CURVE.SPOT($H$2,I61)</f>
+        <v>4.8236509086557806E-2</v>
+      </c>
+      <c r="K61" s="11" cm="1">
+        <f t="array" ref="K61">_xll.FI.CURVE.FORWARD($H$2,I61)</f>
+        <v>4.9162266004027004E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="9:11" x14ac:dyDescent="0.3">
       <c r="I62">
         <v>24</v>
       </c>
-    </row>
-    <row r="63" spans="9:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="J62" s="10" cm="1">
+        <f t="array" ref="J62">_xll.FI.CURVE.SPOT($H$2,I62)</f>
+        <v>4.8255795689005086E-2</v>
+      </c>
+      <c r="K62" s="11" cm="1">
+        <f t="array" ref="K62">_xll.FI.CURVE.FORWARD($H$2,I62)</f>
+        <v>4.9162266004027004E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="9:11" x14ac:dyDescent="0.3">
       <c r="I63">
         <v>24.5</v>
       </c>
-    </row>
-    <row r="64" spans="9:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="J63" s="10" cm="1">
+        <f t="array" ref="J63">_xll.FI.CURVE.SPOT($H$2,I63)</f>
+        <v>4.82742950831892E-2</v>
+      </c>
+      <c r="K63" s="11" cm="1">
+        <f t="array" ref="K63">_xll.FI.CURVE.FORWARD($H$2,I63)</f>
+        <v>4.9162266004027004E-2</v>
+      </c>
+    </row>
+    <row r="64" spans="9:11" x14ac:dyDescent="0.3">
       <c r="I64">
         <v>25</v>
       </c>
-    </row>
-    <row r="65" spans="9:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="J64" s="10" cm="1">
+        <f t="array" ref="J64">_xll.FI.CURVE.SPOT($H$2,I64)</f>
+        <v>4.8292054501605959E-2</v>
+      </c>
+      <c r="K64" s="11" cm="1">
+        <f t="array" ref="K64">_xll.FI.CURVE.FORWARD($H$2,I64)</f>
+        <v>4.9162266004027004E-2</v>
+      </c>
+    </row>
+    <row r="65" spans="9:11" x14ac:dyDescent="0.3">
       <c r="I65">
         <v>25.5</v>
       </c>
-    </row>
-    <row r="66" spans="9:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="J65" s="10" cm="1">
+        <f t="array" ref="J65">_xll.FI.CURVE.SPOT($H$2,I65)</f>
+        <v>4.8309117472241668E-2</v>
+      </c>
+      <c r="K65" s="11" cm="1">
+        <f t="array" ref="K65">_xll.FI.CURVE.FORWARD($H$2,I65)</f>
+        <v>4.9162266004027004E-2</v>
+      </c>
+    </row>
+    <row r="66" spans="9:11" x14ac:dyDescent="0.3">
       <c r="I66">
         <v>26</v>
       </c>
-    </row>
-    <row r="67" spans="9:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="J66" s="10" cm="1">
+        <f t="array" ref="J66">_xll.FI.CURVE.SPOT($H$2,I66)</f>
+        <v>4.8325524174775994E-2</v>
+      </c>
+      <c r="K66" s="11" cm="1">
+        <f t="array" ref="K66">_xll.FI.CURVE.FORWARD($H$2,I66)</f>
+        <v>4.9162266004027004E-2</v>
+      </c>
+    </row>
+    <row r="67" spans="9:11" x14ac:dyDescent="0.3">
       <c r="I67">
         <v>26.5</v>
       </c>
-    </row>
-    <row r="68" spans="9:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="J67" s="10" cm="1">
+        <f t="array" ref="J67">_xll.FI.CURVE.SPOT($H$2,I67)</f>
+        <v>4.8341311756459983E-2</v>
+      </c>
+      <c r="K67" s="11" cm="1">
+        <f t="array" ref="K67">_xll.FI.CURVE.FORWARD($H$2,I67)</f>
+        <v>4.9162266004027004E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="9:11" x14ac:dyDescent="0.3">
       <c r="I68">
         <v>27</v>
       </c>
-    </row>
-    <row r="69" spans="9:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="J68" s="10" cm="1">
+        <f t="array" ref="J68">_xll.FI.CURVE.SPOT($H$2,I68)</f>
+        <v>4.835651461289641E-2</v>
+      </c>
+      <c r="K68" s="11" cm="1">
+        <f t="array" ref="K68">_xll.FI.CURVE.FORWARD($H$2,I68)</f>
+        <v>4.9162266004027004E-2</v>
+      </c>
+    </row>
+    <row r="69" spans="9:11" x14ac:dyDescent="0.3">
       <c r="I69">
         <v>27.5</v>
       </c>
-    </row>
-    <row r="70" spans="9:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="J69" s="10" cm="1">
+        <f t="array" ref="J69">_xll.FI.CURVE.SPOT($H$2,I69)</f>
+        <v>4.837116463818969E-2</v>
+      </c>
+      <c r="K69" s="11" cm="1">
+        <f t="array" ref="K69">_xll.FI.CURVE.FORWARD($H$2,I69)</f>
+        <v>4.9162266004027004E-2</v>
+      </c>
+    </row>
+    <row r="70" spans="9:11" x14ac:dyDescent="0.3">
       <c r="I70">
         <v>28</v>
       </c>
-    </row>
-    <row r="71" spans="9:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="J70" s="10" cm="1">
+        <f t="array" ref="J70">_xll.FI.CURVE.SPOT($H$2,I70)</f>
+        <v>4.8385291448293934E-2</v>
+      </c>
+      <c r="K70" s="11" cm="1">
+        <f t="array" ref="K70">_xll.FI.CURVE.FORWARD($H$2,I70)</f>
+        <v>4.9162266004027004E-2</v>
+      </c>
+    </row>
+    <row r="71" spans="9:11" x14ac:dyDescent="0.3">
       <c r="I71">
         <v>28.5</v>
       </c>
-    </row>
-    <row r="72" spans="9:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="J71" s="10" cm="1">
+        <f t="array" ref="J71">_xll.FI.CURVE.SPOT($H$2,I71)</f>
+        <v>4.8398922580850649E-2</v>
+      </c>
+      <c r="K71" s="11" cm="1">
+        <f t="array" ref="K71">_xll.FI.CURVE.FORWARD($H$2,I71)</f>
+        <v>4.9162266004027004E-2</v>
+      </c>
+    </row>
+    <row r="72" spans="9:11" x14ac:dyDescent="0.3">
       <c r="I72">
         <v>29</v>
       </c>
-    </row>
-    <row r="73" spans="9:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="J72" s="10" cm="1">
+        <f t="array" ref="J72">_xll.FI.CURVE.SPOT($H$2,I72)</f>
+        <v>4.8412083674353693E-2</v>
+      </c>
+      <c r="K72" s="11" cm="1">
+        <f t="array" ref="K72">_xll.FI.CURVE.FORWARD($H$2,I72)</f>
+        <v>4.9162266004027004E-2</v>
+      </c>
+    </row>
+    <row r="73" spans="9:11" x14ac:dyDescent="0.3">
       <c r="I73">
         <v>29.5</v>
       </c>
-    </row>
-    <row r="74" spans="9:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="J73" s="10" cm="1">
+        <f t="array" ref="J73">_xll.FI.CURVE.SPOT($H$2,I73)</f>
+        <v>4.8424798629093914E-2</v>
+      </c>
+      <c r="K73" s="11" cm="1">
+        <f t="array" ref="K73">_xll.FI.CURVE.FORWARD($H$2,I73)</f>
+        <v>4.9162266004027004E-2</v>
+      </c>
+    </row>
+    <row r="74" spans="9:11" x14ac:dyDescent="0.3">
       <c r="I74">
         <v>30</v>
+      </c>
+      <c r="J74" s="10" cm="1">
+        <f t="array" ref="J74">_xll.FI.CURVE.SPOT($H$2,I74)</f>
+        <v>4.8437089752009464E-2</v>
+      </c>
+      <c r="K74" s="11" cm="1">
+        <f t="array" ref="K74">_xll.FI.CURVE.FORWARD($H$2,I74)</f>
+        <v>4.9162266004027004E-2</v>
       </c>
     </row>
   </sheetData>
@@ -2978,6 +5693,7 @@
   <ignoredErrors>
     <ignoredError sqref="C4" formula="1"/>
   </ignoredErrors>
-  <legacyDrawing r:id="rId1"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>